<commit_message>
1. fixed some bug.\n2.add read me document.
</commit_message>
<xml_diff>
--- a/Assets/Demo/Excel/PlayerInfo.xlsx
+++ b/Assets/Demo/Excel/PlayerInfo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -83,6 +83,18 @@
   </si>
   <si>
     <t>May</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isNewPlayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is new player</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -524,7 +536,7 @@
     <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -534,8 +546,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -545,8 +560,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -556,8 +574,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -567,8 +588,11 @@
       <c r="C4">
         <v>10010001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -578,8 +602,11 @@
       <c r="C5">
         <v>10010002</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -589,8 +616,11 @@
       <c r="C6">
         <v>10010003</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -600,8 +630,11 @@
       <c r="C7">
         <v>10010004</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -611,8 +644,11 @@
       <c r="C8">
         <v>10010005</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -622,8 +658,11 @@
       <c r="C9">
         <v>10010006</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -633,8 +672,11 @@
       <c r="C10">
         <v>10010007</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -643,6 +685,9 @@
       </c>
       <c r="C11">
         <v>10010008</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>